<commit_message>
up to apr 30
</commit_message>
<xml_diff>
--- a/McGill RA Working Hours.xlsx
+++ b/McGill RA Working Hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garybi/Desktop/MSc Biostatistics Western/Dr. Marc O. Martel Lab RA/Pain-Research-1-Dr-Marc-O-Martel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DABE8D9-68B3-104C-9C5B-A3DA568ECAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF493DE-885E-1749-8B80-D8755BD8BE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2740" yWindow="2740" windowWidth="21600" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Hours</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>Apr. 16</t>
+  </si>
+  <si>
+    <t>Alice's Data &amp; Plots</t>
+  </si>
+  <si>
+    <t>Apr. 18</t>
+  </si>
+  <si>
+    <t>Meeting (CV)</t>
+  </si>
+  <si>
+    <t>Apr. 23</t>
   </si>
 </sst>
 </file>
@@ -455,7 +467,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -562,6 +574,28 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
may 12 - draft
</commit_message>
<xml_diff>
--- a/McGill RA Working Hours.xlsx
+++ b/McGill RA Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garybi/Desktop/MSc Biostatistics Western/Dr. Marc O. Martel Lab RA/Pain-Research-1-Dr-Marc-O-Martel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF493DE-885E-1749-8B80-D8755BD8BE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C97D34F-6CE0-3C4F-BB63-83961C09588F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2740" yWindow="2740" windowWidth="21600" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Hours</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Apr. 23</t>
+  </si>
+  <si>
+    <t>Recurring meeting</t>
+  </si>
+  <si>
+    <t>May. 7</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -596,35 +602,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
up to may 21
</commit_message>
<xml_diff>
--- a/McGill RA Working Hours.xlsx
+++ b/McGill RA Working Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bijiaqi/Desktop/Project; Daily diaries; 30-days/Pain-Research-1-Dr-Marc-O-Martel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BE06EF-7D98-4B4E-A311-8BCC96C78135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926233FD-29B5-4646-8ABA-2E086C989839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2740" yWindow="2740" windowWidth="21600" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Hours</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -158,7 +158,16 @@
     <t>May. 14</t>
   </si>
   <si>
-    <t>Amount ($)</t>
+    <t>Statistical Analysis (centering, CI, ICC)</t>
+  </si>
+  <si>
+    <t>May. 20</t>
+  </si>
+  <si>
+    <t>May. 21</t>
+  </si>
+  <si>
+    <t>Amount (25$/hour)</t>
   </si>
 </sst>
 </file>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -678,54 +687,76 @@
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C18">
+      <c r="C20">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>17</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C23">
-        <f>SUM(C2:C21)</f>
-        <v>27.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C25">
-        <f>C23*25</f>
-        <v>687.5</v>
+        <f>SUM(C2:C23)</f>
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27">
+        <f>C25*25</f>
+        <v>912.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>